<commit_message>
fix: Correcciones en redaccion
</commit_message>
<xml_diff>
--- a/HU061 Matriz de Pruebas (Traspaso, Fondeo y Movimiento Manual).xlsx
+++ b/HU061 Matriz de Pruebas (Traspaso, Fondeo y Movimiento Manual).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\DNU\Documentacion\HU061 Cuenta Eje SAAS en Prepago SAAS ES\Repo\HU061_Desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragdn\OneDrive\Documentos\Cacao\Requerimientos\HU061 - Cuenta Eje SAAS ES\Desarrollo\HU061_Desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D420BBB-AF17-45FF-B185-AEC5B1806A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F7E9A1-3710-4A7A-86D1-20820C8C058F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ciclo 1" sheetId="3" r:id="rId1"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>Totem</t>
   </si>
@@ -447,15 +447,6 @@
 </t>
   </si>
   <si>
-    <t>1.- Ingresar a Central Administrativa.
-2.- Ir al menú Las Operaciones/Colectivas.
-3.- Seleccionar al cliente considerado para la prueba y revisar la pestaña Cuentas para ver el saldo de la cuenta SaaS.
-4.- Hacer Login en el WebService CacaoParabilia con un usuario y contraseña válidos.
-5.- Utilizar tarjetas origen y destino que pertenezcas al mismo cliente considerado para la prueba.
-6.- Consumir el endpoint TraspasoTarjeta,  para comprobar funcionalidad.
-7.- Consultar nuevamente la colectiva en CA para comprobar que el saldo de la cuenta SaaS no haya sido afectado.</t>
-  </si>
-  <si>
     <t>El traspaso de fondos de una tarjeta a otra, deberá ser permitido siempre y cuando el monto no exceda el saldo de la cuenta origen.
 Así mismo, al ser dos tarjetas de un mismo cliente, la cuenta Saas no será afeactada.</t>
   </si>
@@ -557,6 +548,24 @@
     "DescRespuesta": "Aprobada"
 }</t>
   </si>
+  <si>
+    <t>1.- Ingresar a Central Administrativa.
+2.- Ir al menú Las Operaciones/Colectivas.
+3.- Seleccionar al cliente considerado para la prueba y revisar la pestaña Cuentas para ver el saldo de la cuenta SaaS.
+4.- Hacer Login en el WebService CacaoParabilia con un usuario y contraseña válidos.
+5.- Utilizar tarjetas origen y destino que pertenezcas al mismo cliente considerado para la prueba.
+6.- Consumir el endpoint api/MovimientoManual,  para comprobar funcionalidad.
+7.- Consultar nuevamente la colectiva en CA para comprobar que el saldo de la cuenta SaaS no haya sido afectado.</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a Central Administrativa.
+2.- Ir al menú Las Operaciones/Colectivas.
+3.- Seleccionar al cliente considerado para la prueba y revisar la pestaña Cuentas para ver el saldo de la cuenta SaaS.
+4.- Hacer Login en el WebService CacaoParabilia con un usuario y contraseña válidos.
+5.- Utilizar tarjetas origen y destino que pertenezcas al mismo cliente considerado para la prueba.
+6.- Consumir el endpoint api/FondearTarjeta,  para comprobar funcionalidad.
+7.- Consultar nuevamente la colectiva en CA para comprobar que el saldo de la cuenta SaaS no haya sido afectado.</t>
+  </si>
 </sst>
 </file>
 
@@ -565,7 +574,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -706,6 +715,12 @@
     <font>
       <sz val="10"/>
       <color theme="9" tint="0.39997558519241921"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1003,7 +1018,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1188,6 +1203,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2020,10 +2038,10 @@
   <dimension ref="A1:J843"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2140,13 +2158,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="291.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
+      <c r="A6" s="68">
         <v>1</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
       <c r="D6" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>55</v>
@@ -2158,21 +2176,21 @@
         <v>56</v>
       </c>
       <c r="H6" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="28" t="s">
-        <v>59</v>
-      </c>
       <c r="J6" s="29"/>
     </row>
     <row r="7" spans="1:10" ht="291.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26">
+      <c r="A7" s="68">
         <v>2</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
       <c r="D7" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>55</v>
@@ -2184,21 +2202,21 @@
         <v>56</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" s="29"/>
     </row>
     <row r="8" spans="1:10" ht="291.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26">
+      <c r="A8" s="68">
         <v>3</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
       <c r="D8" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>55</v>
@@ -2207,24 +2225,24 @@
         <v>17</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J8" s="29"/>
     </row>
     <row r="9" spans="1:10" ht="300.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26">
+      <c r="A9" s="68">
         <v>4</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
       <c r="D9" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>55</v>
@@ -2233,24 +2251,24 @@
         <v>17</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:10" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26">
+      <c r="A10" s="68">
         <v>5</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>55</v>
@@ -2259,24 +2277,24 @@
         <v>17</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J10" s="29"/>
     </row>
     <row r="11" spans="1:10" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26">
+      <c r="A11" s="68">
         <v>6</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
       <c r="D11" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="27" t="s">
         <v>55</v>
@@ -2285,13 +2303,13 @@
         <v>17</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" s="29"/>
     </row>

</xml_diff>